<commit_message>
Resolvendo conflito no script_registro.py
</commit_message>
<xml_diff>
--- a/planilha_registro.xlsx
+++ b/planilha_registro.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sicoob-my.sharepoint.com/personal/gabriel_sandres_sicoob_com_br/Documents/Área de Trabalho/versao_final_automacao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Área de Trabalho\automação_visao360\automa-o_visao360_V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_2B59D2BFD360D20D5FFA3611598E60725613FB7D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F01ADB18-3F80-4014-92F8-F95AB4BE2654}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91C8875-9E8A-4E56-826E-49113311498A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Documento do cooperado</t>
   </si>
@@ -41,45 +41,6 @@
   </si>
   <si>
     <t>Observação</t>
-  </si>
-  <si>
-    <t>05534899174</t>
-  </si>
-  <si>
-    <t>WP12345678</t>
-  </si>
-  <si>
-    <t>Pix</t>
-  </si>
-  <si>
-    <t>Dúvida Técnica</t>
-  </si>
-  <si>
-    <t>COB123456789</t>
-  </si>
-  <si>
-    <t>Cobrança Bancária</t>
-  </si>
-  <si>
-    <t>Dúvida Negocial</t>
-  </si>
-  <si>
-    <t>Teste teste teste</t>
-  </si>
-  <si>
-    <t>Poupança</t>
-  </si>
-  <si>
-    <t>Automação para registro</t>
-  </si>
-  <si>
-    <t>Registro 001</t>
-  </si>
-  <si>
-    <t>Conta Corrente</t>
-  </si>
-  <si>
-    <t>Registro 002</t>
   </si>
 </sst>
 </file>
@@ -442,24 +403,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,140 +441,15 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>3179</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>3179</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>3179</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>3179</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>3179</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>3179</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>3179</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{6459b2e0-2ec4-47e6-afc1-6e3f8b684f6a}" enabled="1" method="Privileged" siteId="{b417b620-2ae9-4a83-ab6c-7fbd828bda1d}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>